<commit_message>
Filled Time Spent Per Usecase for first semester
</commit_message>
<xml_diff>
--- a/TimeSpentPerUC.xlsx
+++ b/TimeSpentPerUC.xlsx
@@ -1,42 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Semester 3\FitnessWebAppDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF7B533C-7858-48E3-BB36-3C410F11DE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA0E25A-8FAD-4448-A605-EA04BFA49791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5A931FA6-E660-4B02-BCCE-7F3112D8ED84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>UC</t>
   </si>
@@ -69,19 +53,31 @@
   </si>
   <si>
     <t xml:space="preserve">Edit Exercise </t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -105,6 +101,30 @@
       <right/>
       <top/>
       <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -113,15 +133,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -134,7 +158,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -168,20 +192,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -209,31 +233,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -261,23 +268,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -289,160 +279,186 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0435BE47-18BC-4CE6-BF38-9B2DAA97F351}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,32 +478,122 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <f>23*60/5+11+30+120+150</f>
+        <v>587</v>
+      </c>
+      <c r="D2">
+        <v>270</v>
+      </c>
+      <c r="E2">
+        <f>SUM(B2:D2)/60</f>
+        <v>15.616666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>23*60/5+11+30+150</f>
+        <v>467</v>
+      </c>
+      <c r="D3">
+        <v>270</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="0">SUM(B3:D3)/60</f>
+        <v>12.283333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>120</v>
+      </c>
+      <c r="C4">
+        <f>27*60/5+11+30+120+30+90</f>
+        <v>605</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>12.083333333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>27*60/5+11+30+30+90</f>
+        <v>485</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>8.0833333333333339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="C6">
+        <f>27*60/5+11+30+30+90</f>
+        <v>485</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>8.0833333333333339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <f>120+150+90+540+180</f>
+        <v>1080</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <f>SUM(B2:B7)</f>
+        <v>200</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ref="C8:F8" si="1">SUM(C2:C7)</f>
+        <v>3709</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>540</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>74.150000000000006</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Function Points to existing usecases
</commit_message>
<xml_diff>
--- a/TimeSpentPerUC.xlsx
+++ b/TimeSpentPerUC.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Semester 3\FitnessWebAppDocumentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA0E25A-8FAD-4448-A605-EA04BFA49791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Tabelle1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -64,14 +58,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -88,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -106,15 +107,22 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -122,10 +130,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -133,25 +141,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="14">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -162,10 +201,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -203,71 +242,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -295,7 +334,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -318,11 +357,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -331,13 +370,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -347,7 +386,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -356,7 +395,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -365,7 +404,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -373,10 +412,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -441,156 +480,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="11" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>80</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <f>23*60/5+11+30+120+150</f>
-        <v>587</v>
-      </c>
-      <c r="D2">
+      </c>
+      <c r="D2" s="5">
         <v>270</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <f>SUM(B2:D2)/60</f>
-        <v>15.616666666666667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      </c>
+      <c r="F2" s="7">
+        <v>376.2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="B3" s="7"/>
+      <c r="C3" s="5">
         <f>23*60/5+11+30+150</f>
-        <v>467</v>
-      </c>
-      <c r="D3">
+      </c>
+      <c r="D3" s="5">
         <v>270</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E7" si="0">SUM(B3:D3)/60</f>
-        <v>12.283333333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E3" s="6">
+        <f>SUM(B3:D3)/60</f>
+      </c>
+      <c r="F3" s="7">
+        <v>144.45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>120</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <f>27*60/5+11+30+120+30+90</f>
-        <v>605</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>12.083333333333334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6">
+        <f>SUM(B4:D4)/60</f>
+      </c>
+      <c r="F4" s="7">
+        <v>134.82</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="7"/>
+      <c r="C5" s="5">
         <f>27*60/5+11+30+30+90</f>
-        <v>485</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>8.0833333333333339</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6">
+        <f>SUM(B5:D5)/60</f>
+      </c>
+      <c r="F5" s="7">
+        <v>108.07</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="7"/>
+      <c r="C6" s="5">
         <f>27*60/5+11+30+30+90</f>
-        <v>485</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>8.0833333333333339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6">
+        <f>SUM(B6:D6)/60</f>
+      </c>
+      <c r="F6" s="7">
+        <v>166.92</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="7"/>
+      <c r="C7" s="5">
         <f>120+150+90+540+180</f>
-        <v>1080</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5">
+        <f>SUM(B7:D7)/60</f>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="9">
         <f>SUM(B2:B7)</f>
-        <v>200</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" ref="C8:F8" si="1">SUM(C2:C7)</f>
-        <v>3709</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" si="1"/>
-        <v>540</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="1"/>
-        <v>74.150000000000006</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <f>SUM(C2:C7)</f>
+      </c>
+      <c r="D8" s="9">
+        <f>SUM(D2:D7)</f>
+      </c>
+      <c r="E8" s="10">
+        <f>SUM(E2:E7)</f>
+      </c>
+      <c r="F8" s="9">
+        <f>SUM(F2:F7)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>